<commit_message>
Multilingual Sentiment App Upload
</commit_message>
<xml_diff>
--- a/WebApp/Bar_soup.xlsx
+++ b/WebApp/Bar_soup.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ye.xu2\Ye\Projects\Textmining\Capstone2017Fall\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangyunsi/Desktop/final project/unilever/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="156" yWindow="528" windowWidth="12624" windowHeight="7476"/>
+    <workbookView xWindow="160" yWindow="520" windowWidth="12620" windowHeight="7480"/>
   </bookViews>
   <sheets>
     <sheet name="Women's Informational Survey Hi" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,15 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Women''s Informational Survey Hi'!$A$1:$F$457</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -5487,9 +5495,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -5522,9 +5530,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -5730,20 +5738,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="43.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="36.88671875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="4"/>
+    <col min="5" max="5" width="36.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5763,7 +5771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>33839</v>
       </c>
@@ -5783,7 +5791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>36761</v>
       </c>
@@ -5803,7 +5811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>6756</v>
       </c>
@@ -5823,7 +5831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>16468</v>
       </c>
@@ -5843,7 +5851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>11551</v>
       </c>
@@ -5863,7 +5871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>8548</v>
       </c>
@@ -5883,7 +5891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>21768</v>
       </c>
@@ -5903,7 +5911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>22278</v>
       </c>
@@ -5923,7 +5931,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2210</v>
       </c>
@@ -5943,7 +5951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>24401</v>
       </c>
@@ -5963,7 +5971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>13877</v>
       </c>
@@ -5983,7 +5991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>8355</v>
       </c>
@@ -6003,7 +6011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>29899</v>
       </c>
@@ -6023,7 +6031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>27837</v>
       </c>
@@ -6043,7 +6051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>36854</v>
       </c>
@@ -6063,7 +6071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>35063</v>
       </c>
@@ -6083,7 +6091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1869</v>
       </c>
@@ -6103,7 +6111,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>8010</v>
       </c>
@@ -6123,7 +6131,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>827</v>
       </c>
@@ -6143,7 +6151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>33779</v>
       </c>
@@ -6163,7 +6171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>9532</v>
       </c>
@@ -6183,7 +6191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>12750</v>
       </c>
@@ -6203,7 +6211,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>12002</v>
       </c>
@@ -6223,7 +6231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>36188</v>
       </c>
@@ -6243,7 +6251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>7112</v>
       </c>
@@ -6263,7 +6271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>772</v>
       </c>
@@ -6283,7 +6291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>1235</v>
       </c>
@@ -6303,7 +6311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>33845</v>
       </c>
@@ -6323,7 +6331,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>24044</v>
       </c>
@@ -6343,7 +6351,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28775</v>
       </c>
@@ -6363,7 +6371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>10301</v>
       </c>
@@ -6383,7 +6391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>10070</v>
       </c>
@@ -6403,7 +6411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>27818</v>
       </c>
@@ -6423,7 +6431,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>6238</v>
       </c>
@@ -6443,7 +6451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>32129</v>
       </c>
@@ -6463,7 +6471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>5207</v>
       </c>
@@ -6483,7 +6491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>31692</v>
       </c>
@@ -6503,7 +6511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>35165</v>
       </c>
@@ -6523,7 +6531,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>21802</v>
       </c>
@@ -6543,7 +6551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>2269</v>
       </c>
@@ -6563,7 +6571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>1852</v>
       </c>
@@ -6583,7 +6591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>5818</v>
       </c>
@@ -6603,7 +6611,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>707</v>
       </c>
@@ -6623,7 +6631,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>519</v>
       </c>
@@ -6643,7 +6651,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>22364</v>
       </c>
@@ -6663,7 +6671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>36759</v>
       </c>
@@ -6683,7 +6691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>9582</v>
       </c>
@@ -6703,7 +6711,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>13139</v>
       </c>
@@ -6723,7 +6731,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>36112</v>
       </c>
@@ -6743,7 +6751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>5356</v>
       </c>
@@ -6763,7 +6771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>4046</v>
       </c>
@@ -6783,7 +6791,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>2336</v>
       </c>
@@ -6803,7 +6811,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>34426</v>
       </c>
@@ -6823,7 +6831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>6237</v>
       </c>
@@ -6843,7 +6851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>36227</v>
       </c>
@@ -6863,7 +6871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>15890</v>
       </c>
@@ -6883,7 +6891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>26658</v>
       </c>
@@ -6903,7 +6911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>8575</v>
       </c>
@@ -6923,7 +6931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>31914</v>
       </c>
@@ -6943,7 +6951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>8761</v>
       </c>
@@ -6963,7 +6971,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>2110</v>
       </c>
@@ -6983,7 +6991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>35958</v>
       </c>
@@ -7003,7 +7011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>36629</v>
       </c>
@@ -7023,7 +7031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>8400</v>
       </c>
@@ -7043,7 +7051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>7975</v>
       </c>
@@ -7063,7 +7071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>16186</v>
       </c>
@@ -7083,7 +7091,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>4756</v>
       </c>
@@ -7103,7 +7111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>10420</v>
       </c>
@@ -7123,7 +7131,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>26010</v>
       </c>
@@ -7143,7 +7151,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>35200</v>
       </c>
@@ -7163,7 +7171,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>1783</v>
       </c>
@@ -7183,7 +7191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>27215</v>
       </c>
@@ -7203,7 +7211,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>33755</v>
       </c>
@@ -7223,7 +7231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>19021</v>
       </c>
@@ -7243,7 +7251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>36581</v>
       </c>
@@ -7263,7 +7271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>6332</v>
       </c>
@@ -7283,7 +7291,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>22001</v>
       </c>
@@ -7303,7 +7311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>274</v>
       </c>
@@ -7323,7 +7331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>16493</v>
       </c>
@@ -7343,7 +7351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>34469</v>
       </c>
@@ -7363,7 +7371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>24385</v>
       </c>
@@ -7383,7 +7391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>35355</v>
       </c>
@@ -7403,7 +7411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>21699</v>
       </c>
@@ -7423,7 +7431,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>16521</v>
       </c>
@@ -7443,7 +7451,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="65" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>34901</v>
       </c>
@@ -7463,7 +7471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>18736</v>
       </c>
@@ -7483,7 +7491,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>1397</v>
       </c>
@@ -7503,7 +7511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>10904</v>
       </c>
@@ -7523,7 +7531,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>16519</v>
       </c>
@@ -7543,7 +7551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>6066</v>
       </c>
@@ -7563,7 +7571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>32097</v>
       </c>
@@ -7583,7 +7591,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>18890</v>
       </c>
@@ -7603,7 +7611,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>36708</v>
       </c>
@@ -7623,7 +7631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>912</v>
       </c>
@@ -7643,7 +7651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>26149</v>
       </c>
@@ -7663,7 +7671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>12737</v>
       </c>
@@ -7683,7 +7691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>15621</v>
       </c>
@@ -7703,7 +7711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>34731</v>
       </c>
@@ -7723,7 +7731,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>28761</v>
       </c>
@@ -7743,7 +7751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>2524</v>
       </c>
@@ -7763,7 +7771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>34928</v>
       </c>
@@ -7783,7 +7791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>5643</v>
       </c>
@@ -7803,7 +7811,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>22419</v>
       </c>
@@ -7823,7 +7831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>8280</v>
       </c>
@@ -7843,7 +7851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>23691</v>
       </c>
@@ -7863,7 +7871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>8570</v>
       </c>
@@ -7883,7 +7891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>18469</v>
       </c>
@@ -7903,7 +7911,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>33616</v>
       </c>
@@ -7923,7 +7931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>7545</v>
       </c>
@@ -7943,7 +7951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>13288</v>
       </c>
@@ -7963,7 +7971,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>36038</v>
       </c>
@@ -7983,7 +7991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>36927</v>
       </c>
@@ -8003,7 +8011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>1195</v>
       </c>
@@ -8023,7 +8031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>32983</v>
       </c>
@@ -8043,7 +8051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>36858</v>
       </c>
@@ -8063,7 +8071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>24622</v>
       </c>
@@ -8083,7 +8091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>20006</v>
       </c>
@@ -8103,7 +8111,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>10577</v>
       </c>
@@ -8123,7 +8131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>8385</v>
       </c>
@@ -8143,7 +8151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>26745</v>
       </c>
@@ -8163,7 +8171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>35577</v>
       </c>
@@ -8183,7 +8191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>36925</v>
       </c>
@@ -8203,7 +8211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>30126</v>
       </c>
@@ -8223,7 +8231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>19427</v>
       </c>
@@ -8243,7 +8251,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>32607</v>
       </c>
@@ -8263,7 +8271,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>32264</v>
       </c>
@@ -8283,7 +8291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>12557</v>
       </c>
@@ -8303,7 +8311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>2856</v>
       </c>
@@ -8323,7 +8331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>25019</v>
       </c>
@@ -8343,7 +8351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>31792</v>
       </c>
@@ -8363,7 +8371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>26177</v>
       </c>
@@ -8383,7 +8391,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>35833</v>
       </c>
@@ -8403,7 +8411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>16471</v>
       </c>
@@ -8423,7 +8431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>35592</v>
       </c>
@@ -8443,7 +8451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>36308</v>
       </c>
@@ -8463,7 +8471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>9530</v>
       </c>
@@ -8483,7 +8491,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>29208</v>
       </c>
@@ -8503,7 +8511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>7012</v>
       </c>
@@ -8523,7 +8531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>30475</v>
       </c>
@@ -8543,7 +8551,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>35288</v>
       </c>
@@ -8563,7 +8571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>32533</v>
       </c>
@@ -8583,7 +8591,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>18881</v>
       </c>
@@ -8603,7 +8611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>35024</v>
       </c>
@@ -8623,7 +8631,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>26052</v>
       </c>
@@ -8643,7 +8651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>596</v>
       </c>
@@ -8663,7 +8671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>30773</v>
       </c>
@@ -8683,7 +8691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>26368</v>
       </c>
@@ -8703,7 +8711,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>31707</v>
       </c>
@@ -8723,7 +8731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>31308</v>
       </c>
@@ -8743,7 +8751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>32939</v>
       </c>
@@ -8763,7 +8771,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>5774</v>
       </c>
@@ -8783,7 +8791,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>34437</v>
       </c>
@@ -8803,7 +8811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>1507</v>
       </c>
@@ -8823,7 +8831,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>36347</v>
       </c>
@@ -8843,7 +8851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>32875</v>
       </c>
@@ -8863,7 +8871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>14999</v>
       </c>
@@ -8883,7 +8891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>357</v>
       </c>
@@ -8903,7 +8911,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>5586</v>
       </c>
@@ -8923,7 +8931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>34782</v>
       </c>
@@ -8943,7 +8951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>4033</v>
       </c>
@@ -8963,7 +8971,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>33023</v>
       </c>
@@ -8983,7 +8991,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>31037</v>
       </c>
@@ -9003,7 +9011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>29571</v>
       </c>
@@ -9023,7 +9031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>33780</v>
       </c>
@@ -9043,7 +9051,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>5819</v>
       </c>
@@ -9063,7 +9071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>31600</v>
       </c>
@@ -9083,7 +9091,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>27261</v>
       </c>
@@ -9103,7 +9111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>6502</v>
       </c>
@@ -9123,7 +9131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" ht="65" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>36826</v>
       </c>
@@ -9143,7 +9151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>36520</v>
       </c>
@@ -9163,7 +9171,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>20695</v>
       </c>
@@ -9183,7 +9191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>35384</v>
       </c>
@@ -9203,7 +9211,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>12396</v>
       </c>
@@ -9223,7 +9231,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>15419</v>
       </c>
@@ -9243,7 +9251,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>17946</v>
       </c>
@@ -9263,7 +9271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>2142</v>
       </c>
@@ -9283,7 +9291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>29953</v>
       </c>
@@ -9303,7 +9311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>1673</v>
       </c>
@@ -9323,7 +9331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>25060</v>
       </c>
@@ -9343,7 +9351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>8027</v>
       </c>
@@ -9363,7 +9371,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>32458</v>
       </c>
@@ -9383,7 +9391,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>4937</v>
       </c>
@@ -9403,7 +9411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>11827</v>
       </c>
@@ -9423,7 +9431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>29550</v>
       </c>
@@ -9443,7 +9451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>16389</v>
       </c>
@@ -9463,7 +9471,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>22094</v>
       </c>
@@ -9483,7 +9491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>12820</v>
       </c>
@@ -9503,7 +9511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>2832</v>
       </c>
@@ -9523,7 +9531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>31754</v>
       </c>
@@ -9543,7 +9551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>23893</v>
       </c>
@@ -9563,7 +9571,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>25032</v>
       </c>
@@ -9583,7 +9591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>17094</v>
       </c>
@@ -9603,7 +9611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>36270</v>
       </c>
@@ -9623,7 +9631,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>34932</v>
       </c>
@@ -9643,7 +9651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>14077</v>
       </c>
@@ -9663,7 +9671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>24969</v>
       </c>
@@ -9683,7 +9691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>5832</v>
       </c>
@@ -9703,7 +9711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>11989</v>
       </c>
@@ -9723,7 +9731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>25126</v>
       </c>
@@ -9743,7 +9751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>2037</v>
       </c>
@@ -9763,7 +9771,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
         <v>8109</v>
       </c>
@@ -9783,7 +9791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>36678</v>
       </c>
@@ -9803,7 +9811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>6670</v>
       </c>
@@ -9823,7 +9831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>23658</v>
       </c>
@@ -9843,7 +9851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
         <v>35195</v>
       </c>
@@ -9863,7 +9871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>5369</v>
       </c>
@@ -9883,7 +9891,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
         <v>2632</v>
       </c>
@@ -9903,7 +9911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>32498</v>
       </c>
@@ -9923,7 +9931,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>18679</v>
       </c>
@@ -9943,7 +9951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>3501</v>
       </c>
@@ -9963,7 +9971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>35176</v>
       </c>
@@ -9983,7 +9991,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>36863</v>
       </c>
@@ -10003,7 +10011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>447</v>
       </c>
@@ -10023,7 +10031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>36724</v>
       </c>
@@ -10043,7 +10051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>36747</v>
       </c>
@@ -10063,7 +10071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>16950</v>
       </c>
@@ -10083,7 +10091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>4514</v>
       </c>
@@ -10103,7 +10111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>11151</v>
       </c>
@@ -10123,7 +10131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>22115</v>
       </c>
@@ -10143,7 +10151,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>2788</v>
       </c>
@@ -10163,7 +10171,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>23946</v>
       </c>
@@ -10183,7 +10191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>29855</v>
       </c>
@@ -10203,7 +10211,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>12135</v>
       </c>
@@ -10223,7 +10231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" s="3">
         <v>35227</v>
       </c>
@@ -10243,7 +10251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
         <v>19680</v>
       </c>
@@ -10263,7 +10271,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
         <v>31070</v>
       </c>
@@ -10283,7 +10291,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
         <v>21559</v>
       </c>
@@ -10303,7 +10311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
         <v>24135</v>
       </c>
@@ -10323,7 +10331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
         <v>14551</v>
       </c>
@@ -10343,7 +10351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
         <v>17457</v>
       </c>
@@ -10363,7 +10371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
         <v>24290</v>
       </c>
@@ -10383,7 +10391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
         <v>27571</v>
       </c>
@@ -10403,7 +10411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
         <v>16745</v>
       </c>
@@ -10423,7 +10431,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
         <v>35414</v>
       </c>
@@ -10443,7 +10451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
         <v>8370</v>
       </c>
@@ -10463,7 +10471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
         <v>1622</v>
       </c>
@@ -10483,7 +10491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
         <v>34165</v>
       </c>
@@ -10503,7 +10511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="3">
         <v>32157</v>
       </c>
@@ -10523,7 +10531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
         <v>34279</v>
       </c>
@@ -10543,7 +10551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A241" s="3">
         <v>35964</v>
       </c>
@@ -10563,7 +10571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
         <v>33682</v>
       </c>
@@ -10583,7 +10591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
         <v>28641</v>
       </c>
@@ -10603,7 +10611,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
         <v>12671</v>
       </c>
@@ -10623,7 +10631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
         <v>7349</v>
       </c>
@@ -10643,7 +10651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
         <v>5066</v>
       </c>
@@ -10663,7 +10671,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A247" s="3">
         <v>30585</v>
       </c>
@@ -10683,7 +10691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
         <v>1838</v>
       </c>
@@ -10703,7 +10711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
         <v>36578</v>
       </c>
@@ -10723,7 +10731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
         <v>29591</v>
       </c>
@@ -10743,7 +10751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>34916</v>
       </c>
@@ -10763,7 +10771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
         <v>7085</v>
       </c>
@@ -10783,7 +10791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
         <v>33627</v>
       </c>
@@ -10803,7 +10811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
         <v>28831</v>
       </c>
@@ -10823,7 +10831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
         <v>10483</v>
       </c>
@@ -10843,7 +10851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
         <v>34780</v>
       </c>
@@ -10863,7 +10871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A257" s="3">
         <v>17596</v>
       </c>
@@ -10883,7 +10891,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
         <v>24000</v>
       </c>
@@ -10903,7 +10911,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A259" s="3">
         <v>27231</v>
       </c>
@@ -10923,7 +10931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
         <v>2453</v>
       </c>
@@ -10943,7 +10951,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A261" s="3">
         <v>36396</v>
       </c>
@@ -10963,7 +10971,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
         <v>3709</v>
       </c>
@@ -10983,7 +10991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A263" s="3">
         <v>1349</v>
       </c>
@@ -11003,7 +11011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
         <v>36644</v>
       </c>
@@ -11023,7 +11031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
         <v>19207</v>
       </c>
@@ -11043,7 +11051,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" s="2">
         <v>20111</v>
       </c>
@@ -11063,7 +11071,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
         <v>554</v>
       </c>
@@ -11083,7 +11091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
         <v>1155</v>
       </c>
@@ -11103,7 +11111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
         <v>5051</v>
       </c>
@@ -11123,7 +11131,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="270" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A270" s="2">
         <v>9153</v>
       </c>
@@ -11143,7 +11151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" s="3">
         <v>25223</v>
       </c>
@@ -11163,7 +11171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" s="2">
         <v>28793</v>
       </c>
@@ -11183,7 +11191,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A273" s="3">
         <v>6881</v>
       </c>
@@ -11203,7 +11211,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A274" s="2">
         <v>10031</v>
       </c>
@@ -11223,7 +11231,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
         <v>985</v>
       </c>
@@ -11243,7 +11251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A276" s="2">
         <v>28853</v>
       </c>
@@ -11263,7 +11271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="277" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
         <v>36310</v>
       </c>
@@ -11283,7 +11291,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="278" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278" s="2">
         <v>5612</v>
       </c>
@@ -11303,7 +11311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
         <v>35173</v>
       </c>
@@ -11323,7 +11331,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A280" s="2">
         <v>25763</v>
       </c>
@@ -11343,7 +11351,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281" s="3">
         <v>36551</v>
       </c>
@@ -11363,7 +11371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282" s="2">
         <v>33816</v>
       </c>
@@ -11383,7 +11391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A283" s="3">
         <v>35320</v>
       </c>
@@ -11403,7 +11411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284" s="2">
         <v>28565</v>
       </c>
@@ -11423,7 +11431,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" s="3">
         <v>30446</v>
       </c>
@@ -11443,7 +11451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" s="2">
         <v>16333</v>
       </c>
@@ -11463,7 +11471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A287" s="3">
         <v>20791</v>
       </c>
@@ -11483,7 +11491,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A288" s="2">
         <v>35906</v>
       </c>
@@ -11503,7 +11511,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" s="3">
         <v>34217</v>
       </c>
@@ -11523,7 +11531,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290" s="2">
         <v>21621</v>
       </c>
@@ -11543,7 +11551,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291" s="3">
         <v>6854</v>
       </c>
@@ -11563,7 +11571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A292" s="2">
         <v>30526</v>
       </c>
@@ -11583,7 +11591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A293" s="3">
         <v>25410</v>
       </c>
@@ -11603,7 +11611,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" s="2">
         <v>30338</v>
       </c>
@@ -11623,7 +11631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A295" s="3">
         <v>34879</v>
       </c>
@@ -11643,7 +11651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A296" s="2">
         <v>2436</v>
       </c>
@@ -11663,7 +11671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" s="3">
         <v>5731</v>
       </c>
@@ -11683,7 +11691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" s="2">
         <v>15901</v>
       </c>
@@ -11703,7 +11711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" s="3">
         <v>7521</v>
       </c>
@@ -11723,7 +11731,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A300" s="2">
         <v>22266</v>
       </c>
@@ -11743,7 +11751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A301" s="3">
         <v>29672</v>
       </c>
@@ -11763,7 +11771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A302" s="2">
         <v>32848</v>
       </c>
@@ -11783,7 +11791,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A303" s="3">
         <v>7829</v>
       </c>
@@ -11803,7 +11811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" s="2">
         <v>9300</v>
       </c>
@@ -11823,7 +11831,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A305" s="3">
         <v>16633</v>
       </c>
@@ -11843,7 +11851,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" s="2">
         <v>35468</v>
       </c>
@@ -11863,7 +11871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A307" s="3">
         <v>11333</v>
       </c>
@@ -11883,7 +11891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" s="2">
         <v>21531</v>
       </c>
@@ -11903,7 +11911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A309" s="3">
         <v>13564</v>
       </c>
@@ -11923,7 +11931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" s="2">
         <v>36092</v>
       </c>
@@ -11943,7 +11951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="311" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A311" s="3">
         <v>17885</v>
       </c>
@@ -11963,7 +11971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" s="2">
         <v>9945</v>
       </c>
@@ -11983,7 +11991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" s="3">
         <v>35636</v>
       </c>
@@ -12003,7 +12011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A314" s="2">
         <v>24518</v>
       </c>
@@ -12023,7 +12031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" s="3">
         <v>30345</v>
       </c>
@@ -12043,7 +12051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A316" s="2">
         <v>35099</v>
       </c>
@@ -12063,7 +12071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A317" s="3">
         <v>31701</v>
       </c>
@@ -12083,7 +12091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A318" s="2">
         <v>35409</v>
       </c>
@@ -12103,7 +12111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" s="3">
         <v>32924</v>
       </c>
@@ -12123,7 +12131,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="320" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A320" s="2">
         <v>36864</v>
       </c>
@@ -12143,7 +12151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A321" s="3">
         <v>36947</v>
       </c>
@@ -12163,7 +12171,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" s="2">
         <v>31779</v>
       </c>
@@ -12183,7 +12191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" s="3">
         <v>31273</v>
       </c>
@@ -12203,7 +12211,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" s="2">
         <v>35252</v>
       </c>
@@ -12223,7 +12231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" s="3">
         <v>35568</v>
       </c>
@@ -12243,7 +12251,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326" s="2">
         <v>36568</v>
       </c>
@@ -12263,7 +12271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A327" s="3">
         <v>36632</v>
       </c>
@@ -12283,7 +12291,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A328" s="2">
         <v>35124</v>
       </c>
@@ -12303,7 +12311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A329" s="3">
         <v>12230</v>
       </c>
@@ -12323,7 +12331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A330" s="2">
         <v>30024</v>
       </c>
@@ -12343,7 +12351,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A331" s="3">
         <v>30736</v>
       </c>
@@ -12363,7 +12371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A332" s="2">
         <v>24028</v>
       </c>
@@ -12383,7 +12391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A333" s="3">
         <v>27721</v>
       </c>
@@ -12403,7 +12411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A334" s="2">
         <v>34176</v>
       </c>
@@ -12423,7 +12431,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A335" s="3">
         <v>12505</v>
       </c>
@@ -12443,7 +12451,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A336" s="2">
         <v>7694</v>
       </c>
@@ -12463,7 +12471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="337" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A337" s="3">
         <v>6557</v>
       </c>
@@ -12483,7 +12491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="338" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A338" s="2">
         <v>892</v>
       </c>
@@ -12503,7 +12511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="339" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A339" s="3">
         <v>26244</v>
       </c>
@@ -12523,7 +12531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="340" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A340" s="2">
         <v>31704</v>
       </c>
@@ -12543,7 +12551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A341" s="3">
         <v>23742</v>
       </c>
@@ -12563,7 +12571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A342" s="2">
         <v>14051</v>
       </c>
@@ -12583,7 +12591,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="343" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A343" s="3">
         <v>30608</v>
       </c>
@@ -12603,7 +12611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A344" s="2">
         <v>25437</v>
       </c>
@@ -12623,7 +12631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A345" s="3">
         <v>31331</v>
       </c>
@@ -12643,7 +12651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="346" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A346" s="2">
         <v>11401</v>
       </c>
@@ -12663,7 +12671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347" s="3">
         <v>14055</v>
       </c>
@@ -12683,7 +12691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A348" s="2">
         <v>28691</v>
       </c>
@@ -12703,7 +12711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="349" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A349" s="3">
         <v>32975</v>
       </c>
@@ -12723,7 +12731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="350" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A350" s="2">
         <v>31826</v>
       </c>
@@ -12743,7 +12751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="351" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A351" s="3">
         <v>31590</v>
       </c>
@@ -12763,7 +12771,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A352" s="2">
         <v>7813</v>
       </c>
@@ -12783,7 +12791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A353" s="3">
         <v>23708</v>
       </c>
@@ -12803,7 +12811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="354" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A354" s="2">
         <v>9764</v>
       </c>
@@ -12823,7 +12831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="355" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A355" s="3">
         <v>12021</v>
       </c>
@@ -12843,7 +12851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A356" s="2">
         <v>31556</v>
       </c>
@@ -12863,7 +12871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="357" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A357" s="3">
         <v>31095</v>
       </c>
@@ -12883,7 +12891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A358" s="2">
         <v>2104</v>
       </c>
@@ -12903,7 +12911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A359" s="3">
         <v>19387</v>
       </c>
@@ -12923,7 +12931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A360" s="2">
         <v>1578</v>
       </c>
@@ -12943,7 +12951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A361" s="3">
         <v>24984</v>
       </c>
@@ -12963,7 +12971,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A362" s="2">
         <v>16813</v>
       </c>
@@ -12983,7 +12991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A363" s="3">
         <v>17385</v>
       </c>
@@ -13003,7 +13011,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A364" s="2">
         <v>13473</v>
       </c>
@@ -13023,7 +13031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A365" s="3">
         <v>1297</v>
       </c>
@@ -13043,7 +13051,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="366" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A366" s="2">
         <v>8908</v>
       </c>
@@ -13063,7 +13071,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="367" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A367" s="3">
         <v>20253</v>
       </c>
@@ -13083,7 +13091,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A368" s="2">
         <v>16294</v>
       </c>
@@ -13103,7 +13111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="369" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A369" s="3">
         <v>17277</v>
       </c>
@@ -13123,7 +13131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="370" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A370" s="2">
         <v>26629</v>
       </c>
@@ -13143,7 +13151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A371" s="3">
         <v>26058</v>
       </c>
@@ -13163,7 +13171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A372" s="2">
         <v>6138</v>
       </c>
@@ -13183,7 +13191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" ht="65" x14ac:dyDescent="0.2">
       <c r="A373" s="3">
         <v>13667</v>
       </c>
@@ -13203,7 +13211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="374" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A374" s="2">
         <v>11430</v>
       </c>
@@ -13223,7 +13231,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="375" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A375" s="3">
         <v>24637</v>
       </c>
@@ -13243,7 +13251,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A376" s="2">
         <v>27039</v>
       </c>
@@ -13263,7 +13271,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A377" s="3">
         <v>25385</v>
       </c>
@@ -13283,7 +13291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A378" s="2">
         <v>12487</v>
       </c>
@@ -13303,7 +13311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="379" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A379" s="3">
         <v>17404</v>
       </c>
@@ -13323,7 +13331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A380" s="2">
         <v>163</v>
       </c>
@@ -13343,7 +13351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A381" s="3">
         <v>3458</v>
       </c>
@@ -13363,7 +13371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A382" s="2">
         <v>23458</v>
       </c>
@@ -13383,7 +13391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A383" s="3">
         <v>3960</v>
       </c>
@@ -13403,7 +13411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="384" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A384" s="2">
         <v>1802</v>
       </c>
@@ -13423,7 +13431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="385" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A385" s="3">
         <v>9036</v>
       </c>
@@ -13443,7 +13451,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A386" s="2">
         <v>22930</v>
       </c>
@@ -13463,7 +13471,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="387" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:6" ht="65" x14ac:dyDescent="0.2">
       <c r="A387" s="3">
         <v>8367</v>
       </c>
@@ -13483,7 +13491,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="388" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A388" s="2">
         <v>8394</v>
       </c>
@@ -13503,7 +13511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="389" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A389" s="3">
         <v>21882</v>
       </c>
@@ -13523,7 +13531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A390" s="2">
         <v>16198</v>
       </c>
@@ -13543,7 +13551,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="391" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A391" s="3">
         <v>17417</v>
       </c>
@@ -13563,7 +13571,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A392" s="2">
         <v>22459</v>
       </c>
@@ -13583,7 +13591,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="393" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A393" s="3">
         <v>2653</v>
       </c>
@@ -13603,7 +13611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="394" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A394" s="2">
         <v>20584</v>
       </c>
@@ -13623,7 +13631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="395" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A395" s="3">
         <v>9391</v>
       </c>
@@ -13643,7 +13651,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A396" s="2">
         <v>11612</v>
       </c>
@@ -13663,7 +13671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A397" s="3">
         <v>21988</v>
       </c>
@@ -13683,7 +13691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="398" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A398" s="2">
         <v>12537</v>
       </c>
@@ -13703,7 +13711,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="399" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A399" s="3">
         <v>21326</v>
       </c>
@@ -13723,7 +13731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="400" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A400" s="2">
         <v>18741</v>
       </c>
@@ -13743,7 +13751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="401" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A401" s="3">
         <v>11208</v>
       </c>
@@ -13763,7 +13771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A402" s="2">
         <v>18260</v>
       </c>
@@ -13783,7 +13791,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A403" s="3">
         <v>7191</v>
       </c>
@@ -13803,7 +13811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A404" s="2">
         <v>12722</v>
       </c>
@@ -13823,7 +13831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="405" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A405" s="3">
         <v>12267</v>
       </c>
@@ -13843,7 +13851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="406" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A406" s="2">
         <v>15208</v>
       </c>
@@ -13863,7 +13871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="407" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A407" s="3">
         <v>7427</v>
       </c>
@@ -13883,7 +13891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A408" s="2">
         <v>16952</v>
       </c>
@@ -13903,7 +13911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A409" s="3">
         <v>17433</v>
       </c>
@@ -13923,7 +13931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="410" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A410" s="2">
         <v>1298</v>
       </c>
@@ -13943,7 +13951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A411" s="3">
         <v>17504</v>
       </c>
@@ -13963,7 +13971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A412" s="2">
         <v>11533</v>
       </c>
@@ -13983,7 +13991,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="413" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A413" s="3">
         <v>16193</v>
       </c>
@@ -14003,7 +14011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="414" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A414" s="2">
         <v>13127</v>
       </c>
@@ -14023,7 +14031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A415" s="3">
         <v>11641</v>
       </c>
@@ -14043,7 +14051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="416" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A416" s="2">
         <v>270</v>
       </c>
@@ -14063,7 +14071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A417" s="3">
         <v>12088</v>
       </c>
@@ -14083,7 +14091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A418" s="2">
         <v>5910</v>
       </c>
@@ -14103,7 +14111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A419" s="3">
         <v>10263</v>
       </c>
@@ -14123,7 +14131,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="420" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A420" s="2">
         <v>12367</v>
       </c>
@@ -14143,7 +14151,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="421" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A421" s="3">
         <v>13934</v>
       </c>
@@ -14163,7 +14171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="422" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A422" s="2">
         <v>5935</v>
       </c>
@@ -14183,7 +14191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="423" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A423" s="3">
         <v>1511</v>
       </c>
@@ -14203,7 +14211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A424" s="2">
         <v>13827</v>
       </c>
@@ -14223,7 +14231,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="425" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A425" s="3">
         <v>7140</v>
       </c>
@@ -14243,7 +14251,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="426" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A426" s="2">
         <v>11046</v>
       </c>
@@ -14263,7 +14271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="427" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A427" s="3">
         <v>6182</v>
       </c>
@@ -14283,7 +14291,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="428" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A428" s="2">
         <v>3465</v>
       </c>
@@ -14303,7 +14311,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="429" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A429" s="3">
         <v>11719</v>
       </c>
@@ -14323,7 +14331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="430" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A430" s="2">
         <v>8672</v>
       </c>
@@ -14343,7 +14351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A431" s="3">
         <v>12520</v>
       </c>
@@ -14363,7 +14371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="432" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A432" s="2">
         <v>9093</v>
       </c>
@@ -14383,7 +14391,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A433" s="3">
         <v>847</v>
       </c>
@@ -14403,7 +14411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A434" s="2">
         <v>1608</v>
       </c>
@@ -14423,7 +14431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="435" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A435" s="3">
         <v>7824</v>
       </c>
@@ -14443,7 +14451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="436" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A436" s="2">
         <v>7304</v>
       </c>
@@ -14463,7 +14471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A437" s="3">
         <v>1751</v>
       </c>
@@ -14483,7 +14491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="438" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A438" s="2">
         <v>7504</v>
       </c>
@@ -14503,7 +14511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="439" spans="1:6" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:6" ht="78" x14ac:dyDescent="0.2">
       <c r="A439" s="3">
         <v>5177</v>
       </c>
@@ -14523,7 +14531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="440" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A440" s="2">
         <v>1679</v>
       </c>
@@ -14543,7 +14551,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="441" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A441" s="3">
         <v>3466</v>
       </c>
@@ -14563,7 +14571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="442" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A442" s="2">
         <v>3445</v>
       </c>
@@ -14583,7 +14591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A443" s="3">
         <v>713</v>
       </c>
@@ -14603,7 +14611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="444" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A444" s="2">
         <v>1248</v>
       </c>
@@ -14623,7 +14631,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A445" s="3">
         <v>4096</v>
       </c>
@@ -14643,7 +14651,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="446" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A446" s="2">
         <v>2838</v>
       </c>
@@ -14663,7 +14671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="447" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A447" s="3">
         <v>2088</v>
       </c>
@@ -14683,7 +14691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="448" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A448" s="2">
         <v>1928</v>
       </c>
@@ -14703,7 +14711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="449" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A449" s="3">
         <v>1900</v>
       </c>
@@ -14723,7 +14731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="450" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A450" s="2">
         <v>1446</v>
       </c>
@@ -14743,7 +14751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A451" s="3">
         <v>3958</v>
       </c>
@@ -14763,7 +14771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="452" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A452" s="2">
         <v>3626</v>
       </c>
@@ -14783,7 +14791,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A453" s="3">
         <v>644</v>
       </c>
@@ -14803,7 +14811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="454" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A454" s="2">
         <v>3223</v>
       </c>
@@ -14823,7 +14831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="455" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A455" s="3">
         <v>2215</v>
       </c>
@@ -14843,7 +14851,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A456" s="2">
         <v>629</v>
       </c>
@@ -14863,7 +14871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="457" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A457" s="3">
         <v>216</v>
       </c>

</xml_diff>